<commit_message>
Adicionado as tabelas de método de pagamento, pagamentos e assinaturas
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57835071-1E1F-40FA-B72A-6964AF99D8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25670084-BFF9-44FE-B304-9B0CC3BE37C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
     <sheet name="plan_modalities" sheetId="2" r:id="rId2"/>
+    <sheet name="subscriptions" sheetId="3" r:id="rId3"/>
+    <sheet name="payments" sheetId="4" r:id="rId4"/>
+    <sheet name="payment_method" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
   <si>
     <t>Tabela</t>
   </si>
@@ -164,13 +167,103 @@
   </si>
   <si>
     <t>id_modalities</t>
+  </si>
+  <si>
+    <t>subscriptions</t>
+  </si>
+  <si>
+    <t>id_subscriptions</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados das assinaturas dos alunos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador da assinatura </t>
+  </si>
+  <si>
+    <t>id_user</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>dt_start</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>0 a 1</t>
+  </si>
+  <si>
+    <t>1000-01-01 a 9999-12-31</t>
+  </si>
+  <si>
+    <t>Código de identificador do usuário</t>
+  </si>
+  <si>
+    <t>Verificar se assinatura está ativa ou não</t>
+  </si>
+  <si>
+    <t>Data que foi feita a assinatura</t>
+  </si>
+  <si>
+    <t>payments</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados dos pagamentos.</t>
+  </si>
+  <si>
+    <t>id_payment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do pagamento </t>
+  </si>
+  <si>
+    <t>Código de identificador da assinatura</t>
+  </si>
+  <si>
+    <t>dt_payment</t>
+  </si>
+  <si>
+    <t>Data que foi feito o pagamento</t>
+  </si>
+  <si>
+    <t>Preço da assinatura</t>
+  </si>
+  <si>
+    <t>id_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do método de pagamento </t>
+  </si>
+  <si>
+    <t>name_method</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>1 a 20</t>
+  </si>
+  <si>
+    <t>Nome do método de pagamento</t>
+  </si>
+  <si>
+    <t>payment_method</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados dos métodos de pagamentos.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,6 +282,14 @@
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -278,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -304,34 +405,82 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +798,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,47 +813,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -725,14 +874,14 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -747,10 +896,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
@@ -767,10 +916,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -785,17 +934,17 @@
       <c r="H7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="11"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -808,14 +957,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
@@ -828,22 +977,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
@@ -853,65 +1002,65 @@
       <c r="E11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="16"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="16"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="16"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="16"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A15:B15"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="F15:H15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -922,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1B2A90-2EDE-4106-8464-F104942A32C4}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,47 +1087,47 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -999,14 +1148,14 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E5" s="3" t="s">
@@ -1021,14 +1170,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1041,23 +1190,23 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1067,60 +1216,66 @@
       <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="18"/>
+      <c r="H30" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A9:B9"/>
@@ -1129,6 +1284,772 @@
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B329C7B-0515-40D2-8749-7CF9ED1A5F1F}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1D4592-C439-470F-808C-04884423AC9E}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD34664-5E0B-41BB-B6D6-88BEB2F44BAE}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="38"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F8:H8"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>

</xml_diff>

<commit_message>
Adicionado as tabelas de modalidades, instrutor da modalidade, aulas e usuários. Ainda não foi adicionado os índices, vou verificar depois tambem as chaves estrangeiras
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25670084-BFF9-44FE-B304-9B0CC3BE37C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3C0B2-1468-4C33-9FA6-8E4FB8D112DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="subscriptions" sheetId="3" r:id="rId3"/>
     <sheet name="payments" sheetId="4" r:id="rId4"/>
     <sheet name="payment_method" sheetId="5" r:id="rId5"/>
+    <sheet name="modalities" sheetId="6" r:id="rId6"/>
+    <sheet name="instructor_modalities" sheetId="7" r:id="rId7"/>
+    <sheet name="classes" sheetId="8" r:id="rId8"/>
+    <sheet name="users" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="121">
   <si>
     <t>Tabela</t>
   </si>
@@ -257,6 +261,150 @@
   </si>
   <si>
     <t>Tabela responsável por armazenar os dados dos métodos de pagamentos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> d</t>
+  </si>
+  <si>
+    <t>modalities</t>
+  </si>
+  <si>
+    <t>smallint</t>
+  </si>
+  <si>
+    <t>-32.768 a 32.767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador da modalidade </t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados das modalidades.</t>
+  </si>
+  <si>
+    <t>Nome da modalidade</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Descrição da modalidade</t>
+  </si>
+  <si>
+    <t>instructor_modalities</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados de qual modalidade vai ser ensinada por um determinado instrutor .</t>
+  </si>
+  <si>
+    <t>id_instructor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do instructor </t>
+  </si>
+  <si>
+    <t>classes</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados das aulas</t>
+  </si>
+  <si>
+    <t>id_class</t>
+  </si>
+  <si>
+    <t>Código de identificador da aula</t>
+  </si>
+  <si>
+    <t>Código de identificador do instrutor</t>
+  </si>
+  <si>
+    <t>dt_hour_class</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>Data e hora da aula</t>
+  </si>
+  <si>
+    <t>1000-01-01 00:00:00 a 9999-12-31 23:59:59</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados dos usuários.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do usuário </t>
+  </si>
+  <si>
+    <t>nm_user</t>
+  </si>
+  <si>
+    <t>Nome do usuário</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>1 a 100</t>
+  </si>
+  <si>
+    <t>E-mail do usuário</t>
+  </si>
+  <si>
+    <t>password_hash</t>
+  </si>
+  <si>
+    <t>Senha do usuário</t>
+  </si>
+  <si>
+    <t>Verificar se usuário está ativo ou não</t>
+  </si>
+  <si>
+    <t>dt_creation</t>
+  </si>
+  <si>
+    <t>Data e hora da criação do usuário</t>
+  </si>
+  <si>
+    <t>dt_birth</t>
+  </si>
+  <si>
+    <t>Data de nascimento do usuário</t>
+  </si>
+  <si>
+    <t>specialty</t>
+  </si>
+  <si>
+    <t>A especialidade do usuário</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>mediumint</t>
+  </si>
+  <si>
+    <t>-8.388.608 a 8.388.607</t>
+  </si>
+  <si>
+    <t>Número de telefone do usuário</t>
+  </si>
+  <si>
+    <t>id_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do endereço </t>
+  </si>
+  <si>
+    <t>id_user_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do tipo do usuário </t>
   </si>
 </sst>
 </file>
@@ -379,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -434,9 +582,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -452,27 +597,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -481,6 +609,47 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,7 +967,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,47 +982,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -874,10 +1043,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -896,10 +1065,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
@@ -916,10 +1085,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -937,10 +1106,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -957,10 +1126,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1039,28 +1208,28 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1087,47 +1256,47 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1148,10 +1317,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1170,10 +1339,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1223,44 +1392,44 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1270,12 +1439,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A9:B9"/>
@@ -1284,6 +1447,12 @@
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1295,7 +1464,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,47 +1479,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1371,10 +1540,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1393,10 +1562,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
@@ -1413,63 +1582,63 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="32" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32" t="s">
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="35" t="s">
+      <c r="E8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="27" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32" t="s">
+      <c r="E9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1499,21 +1668,21 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1550,18 +1719,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1572,7 +1741,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,47 +1756,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1648,10 +1817,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1670,10 +1839,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1690,63 +1859,63 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="32" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32" t="s">
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
         <v>63</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="38"/>
+      <c r="C8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="35" t="s">
+      <c r="E8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="27" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="32" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="37" t="s">
+      <c r="E9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="29" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1776,21 +1945,21 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1827,18 +1996,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1846,10 +2015,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD34664-5E0B-41BB-B6D6-88BEB2F44BAE}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,47 +2033,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="20"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1925,10 +2094,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="18"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1947,10 +2116,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="18"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
@@ -1993,11 +2162,11 @@
       <c r="E8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -2040,11 +2209,16 @@
       <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="38"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
     </row>
   </sheetData>
@@ -2060,4 +2234,1117 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88679C7A-C2BB-41E9-BAAB-56A3F29E0F7C}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="43"/>
+      <c r="H9" s="44"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92DFA70-0B24-4FEB-931D-B25A069BE1F6}">
+  <dimension ref="A1:L30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="22"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C10CCC63-B6F6-46BF-9364-1328450D0C7A}">
+  <dimension ref="A1:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="32"/>
+      <c r="C7" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="13"/>
+      <c r="C10" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1765648-80F5-4C79-B471-51305D7461D1}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34"/>
+      <c r="C4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="36"/>
+      <c r="C9" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" s="36"/>
+      <c r="C10" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="36"/>
+      <c r="C11" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="36"/>
+      <c r="C15" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="44"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="39"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="40"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado as ultimas tabelas, tipos de usuário, endereços e número de telefone, vou verificar agora os índices
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA3C0B2-1468-4C33-9FA6-8E4FB8D112DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7473B806-3631-4DC1-B401-A422536DFA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="11" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
     <sheet name="instructor_modalities" sheetId="7" r:id="rId7"/>
     <sheet name="classes" sheetId="8" r:id="rId8"/>
     <sheet name="users" sheetId="9" r:id="rId9"/>
+    <sheet name="user_types" sheetId="10" r:id="rId10"/>
+    <sheet name="address" sheetId="11" r:id="rId11"/>
+    <sheet name="phone" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="149">
   <si>
     <t>Tabela</t>
   </si>
@@ -405,6 +408,90 @@
   </si>
   <si>
     <t xml:space="preserve">Código de identificador do tipo do usuário </t>
+  </si>
+  <si>
+    <t>user_types</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados dos tipos de usuário.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do tipo de usuário </t>
+  </si>
+  <si>
+    <t>Nome do tipo de usuário</t>
+  </si>
+  <si>
+    <t>Descrição sobre o tipo de usuário</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados de endereços.</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>Nome da rua</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Localização do endereço</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>Número da casa</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>Ponto de referência para achar a casa</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Cidade do endereço</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Estado do endereço</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>País do endereço</t>
+  </si>
+  <si>
+    <t>Tabela responsável por armazenar os dados do telefone dos usuários.</t>
+  </si>
+  <si>
+    <t>id_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do telefone </t>
+  </si>
+  <si>
+    <t>nr_telefone</t>
+  </si>
+  <si>
+    <t>varchar(15)</t>
+  </si>
+  <si>
+    <t>1 a 15</t>
+  </si>
+  <si>
+    <t>Número do telefone</t>
   </si>
 </sst>
 </file>
@@ -527,7 +614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -616,9 +703,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -646,9 +754,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -982,47 +1087,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1043,10 +1148,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1065,10 +1170,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1085,10 +1190,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1106,10 +1211,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1126,10 +1231,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1208,31 +1313,821 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="31"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B0D3FAD-57DC-479F-B27B-AAF57A04ED9E}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="13"/>
+      <c r="C9" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="50"/>
+      <c r="H9" s="51"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="34"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="35"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FE0885-18EC-424D-8A59-3E6F1F5E97D1}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="43"/>
+      <c r="C7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="43"/>
+      <c r="C8" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="43"/>
+      <c r="C9" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="45"/>
+      <c r="C12" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="50"/>
+      <c r="H14" s="51"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="34"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="35"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1AA6A6-CB8B-4065-8215-EA9657872912}">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="10"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="34"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="30"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
@@ -1256,47 +2151,47 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1317,10 +2212,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1339,10 +2234,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -1392,44 +2287,44 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1439,6 +2334,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A9:B9"/>
@@ -1447,12 +2348,6 @@
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1464,7 +2359,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,47 +2374,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1540,10 +2435,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1562,10 +2457,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
@@ -1582,10 +2477,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="26" t="s">
         <v>8</v>
       </c>
@@ -1603,10 +2498,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="21" t="s">
         <v>49</v>
       </c>
@@ -1623,10 +2518,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="26" t="s">
         <v>51</v>
       </c>
@@ -1668,21 +2563,21 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="40"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1719,18 +2614,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F11:H11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1741,7 +2636,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1756,47 +2651,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -1817,10 +2712,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1839,10 +2734,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
@@ -1859,10 +2754,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="26" t="s">
         <v>51</v>
       </c>
@@ -1880,10 +2775,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="21" t="s">
         <v>32</v>
       </c>
@@ -1900,10 +2795,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="26" t="s">
         <v>8</v>
       </c>
@@ -1945,21 +2840,21 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="4"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="40"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1996,18 +2891,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2033,47 +2928,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2094,10 +2989,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2116,10 +3011,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
@@ -2162,11 +3057,11 @@
       <c r="E8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -2256,47 +3151,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -2317,10 +3212,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="18" t="s">
         <v>75</v>
       </c>
@@ -2339,10 +3234,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
@@ -2359,10 +3254,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="26" t="s">
         <v>11</v>
       </c>
@@ -2405,11 +3300,11 @@
       <c r="E9" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
@@ -2473,10 +3368,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92DFA70-0B24-4FEB-931D-B25A069BE1F6}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2491,47 +3386,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -2552,10 +3447,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -2574,10 +3469,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="18" t="s">
         <v>75</v>
       </c>
@@ -2620,11 +3515,11 @@
       <c r="E8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
@@ -2671,12 +3566,7 @@
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
     </row>
   </sheetData>
@@ -2713,47 +3603,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -2774,10 +3664,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -2796,10 +3686,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="18" t="s">
         <v>75</v>
       </c>
@@ -2816,10 +3706,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="38"/>
       <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
@@ -2837,10 +3727,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="38"/>
       <c r="C8" s="18" t="s">
         <v>92</v>
       </c>
@@ -2919,14 +3809,14 @@
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="31"/>
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="4"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -2950,8 +3840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1765648-80F5-4C79-B471-51305D7461D1}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2966,47 +3856,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -3027,10 +3917,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="38"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -3049,10 +3939,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
@@ -3069,10 +3959,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="42" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="36"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="26" t="s">
         <v>101</v>
       </c>
@@ -3090,10 +3980,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="45"/>
       <c r="C8" s="21" t="s">
         <v>11</v>
       </c>
@@ -3110,10 +4000,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="36"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="26" t="s">
         <v>49</v>
       </c>
@@ -3130,10 +4020,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="36"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="26" t="s">
         <v>92</v>
       </c>
@@ -3149,11 +4039,11 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+    <row r="11" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="36"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="26" t="s">
         <v>51</v>
       </c>
@@ -3170,10 +4060,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="38"/>
+      <c r="B12" s="45"/>
       <c r="C12" s="21" t="s">
         <v>24</v>
       </c>
@@ -3189,11 +4079,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+    <row r="13" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="36"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="26" t="s">
         <v>114</v>
       </c>
@@ -3209,11 +4099,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
+    <row r="14" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="36"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="26" t="s">
         <v>114</v>
       </c>
@@ -3229,11 +4119,11 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="45" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="36"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="26" t="s">
         <v>8</v>
       </c>
@@ -3275,21 +4165,21 @@
       <c r="E17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="44"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="51"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="4"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="40"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
@@ -3326,11 +4216,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="F18:H18"/>
@@ -3338,12 +4229,11 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Esqueci de trocar o arquivo, agora sim, botei alguns indices
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7473B806-3631-4DC1-B401-A422536DFA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD5FC14-B15A-491B-AAC1-506A2D7DC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="11" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="162">
   <si>
     <t>Tabela</t>
   </si>
@@ -492,6 +492,45 @@
   </si>
   <si>
     <t>Número do telefone</t>
+  </si>
+  <si>
+    <t>city, state, country</t>
+  </si>
+  <si>
+    <t>idx_address_city_state_country</t>
+  </si>
+  <si>
+    <t>idx_phone_nr</t>
+  </si>
+  <si>
+    <t>nr_phone</t>
+  </si>
+  <si>
+    <t>idx_users_email</t>
+  </si>
+  <si>
+    <t>idx_users_types_name</t>
+  </si>
+  <si>
+    <t>idx_users_dt_creation</t>
+  </si>
+  <si>
+    <t>idx_users_user_type</t>
+  </si>
+  <si>
+    <t>idx_users_address</t>
+  </si>
+  <si>
+    <t>idx_modalities_name</t>
+  </si>
+  <si>
+    <t>idx_instr_mod_instructor</t>
+  </si>
+  <si>
+    <t>idx_instr_mod_modality</t>
+  </si>
+  <si>
+    <t>idx_plans_name</t>
   </si>
 </sst>
 </file>
@@ -614,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -711,12 +750,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -724,9 +766,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -753,6 +792,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,47 +1135,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1148,10 +1196,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1170,10 +1218,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1190,10 +1238,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1211,10 +1259,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1231,10 +1279,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1283,14 +1331,20 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="46" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="47"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15"/>
+      <c r="F12" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -1313,28 +1367,30 @@
       <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="38"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1346,7 +1402,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,47 +1417,47 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="33" t="s">
         <v>4</v>
       </c>
@@ -1422,10 +1478,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="32" t="s">
         <v>8</v>
       </c>
@@ -1444,10 +1500,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="32" t="s">
         <v>24</v>
       </c>
@@ -1517,52 +1573,33 @@
       <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="31"/>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="35"/>
-    </row>
+      <c r="F10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="B1:H1"/>
@@ -1578,10 +1615,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45FE0885-18EC-424D-8A59-3E6F1F5E97D1}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,47 +1633,47 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="33" t="s">
         <v>4</v>
       </c>
@@ -1657,10 +1694,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="32" t="s">
         <v>114</v>
       </c>
@@ -1679,10 +1716,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="32" t="s">
         <v>11</v>
       </c>
@@ -1852,50 +1889,35 @@
       <c r="H14" s="51"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="38"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="35"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="35"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="35"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="34"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="35"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="D15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="15">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
@@ -1903,12 +1925,6 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1918,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1AA6A6-CB8B-4065-8215-EA9657872912}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,47 +1950,47 @@
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="33" t="s">
         <v>4</v>
       </c>
@@ -1995,10 +2011,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="32" t="s">
         <v>114</v>
       </c>
@@ -2017,10 +2033,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="32" t="s">
         <v>146</v>
       </c>
@@ -2070,45 +2086,23 @@
       <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="34" t="s">
+        <v>151</v>
+      </c>
       <c r="B9" s="35"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="31"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="31"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="35"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="35"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="35"/>
-    </row>
+      <c r="F9" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I13" s="30"/>
     </row>
@@ -2118,7 +2112,8 @@
       <c r="H30" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -2151,47 +2146,47 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2212,10 +2207,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2234,10 +2229,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2287,44 +2282,44 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2334,12 +2329,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="A9:B9"/>
@@ -2348,6 +2337,12 @@
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2374,47 +2369,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2435,10 +2430,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2457,10 +2452,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
@@ -2614,18 +2609,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2651,47 +2646,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2712,10 +2707,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2734,10 +2729,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
@@ -2891,18 +2886,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2928,47 +2923,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2989,10 +2984,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -3011,10 +3006,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
@@ -3136,7 +3131,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3151,47 +3146,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -3212,10 +3207,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="18" t="s">
         <v>75</v>
       </c>
@@ -3234,10 +3229,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
@@ -3307,52 +3302,33 @@
       <c r="H9" s="51"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="46" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-    </row>
+      <c r="F10" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="B1:H1"/>
@@ -3371,7 +3347,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3386,47 +3362,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -3447,10 +3423,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -3469,10 +3445,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="18" t="s">
         <v>75</v>
       </c>
@@ -3522,45 +3498,39 @@
       <c r="H8" s="51"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="46" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="47"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="20"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="20"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="24"/>
+      <c r="F9" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="48"/>
+      <c r="H9" s="47"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="47"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="20"/>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="20"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="24"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
-    </row>
+      <c r="F10" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I13" s="30"/>
     </row>
@@ -3570,7 +3540,11 @@
       <c r="H30" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A10:B10"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -3603,47 +3577,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -3664,10 +3638,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -3686,10 +3660,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="18" t="s">
         <v>75</v>
       </c>
@@ -3706,10 +3680,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
@@ -3727,10 +3701,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="18" t="s">
         <v>92</v>
       </c>
@@ -3809,14 +3783,14 @@
       <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
       <c r="C14" s="4"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -3840,8 +3814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1765648-80F5-4C79-B471-51305D7461D1}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3856,47 +3830,47 @@
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="40"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="19" t="s">
         <v>4</v>
       </c>
@@ -3917,10 +3891,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="38"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="18" t="s">
         <v>8</v>
       </c>
@@ -3939,10 +3913,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="38"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
@@ -4039,7 +4013,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
         <v>109</v>
       </c>
@@ -4079,7 +4053,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>113</v>
       </c>
@@ -4099,7 +4073,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42" t="s">
         <v>117</v>
       </c>
@@ -4119,7 +4093,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="37" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="42" t="s">
         <v>119</v>
       </c>
@@ -4172,56 +4146,83 @@
       <c r="H17" s="51"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
+      <c r="A18" s="46" t="s">
+        <v>153</v>
+      </c>
       <c r="B18" s="47"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="20"/>
+      <c r="D18" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E18" s="20"/>
-      <c r="F18" s="46"/>
+      <c r="F18" s="46" t="s">
+        <v>100</v>
+      </c>
       <c r="G18" s="48"/>
       <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="46" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="47"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="20"/>
+      <c r="D19" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E19" s="20"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="24"/>
+      <c r="F19" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" s="48"/>
+      <c r="H19" s="47"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="46" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="47"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="20"/>
+      <c r="D20" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E20" s="20"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="24"/>
+      <c r="F20" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="48"/>
+      <c r="H20" s="47"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="46" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="47"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="20"/>
+      <c r="D21" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E21" s="20"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="24"/>
+      <c r="F21" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="48"/>
+      <c r="H21" s="47"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H30" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
+  <mergeCells count="24">
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A19:B19"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="F18:H18"/>
@@ -4231,9 +4232,12 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Arquivo com todos os indices
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD5FC14-B15A-491B-AAC1-506A2D7DC644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9671C69B-DF93-4A23-98F8-7CD25F9E49CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="11" xr2:uid="{8A75A3C3-1CC3-42DF-908E-18684CFF6B01}"/>
   </bookViews>
   <sheets>
     <sheet name="plans" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="174">
   <si>
     <t>Tabela</t>
   </si>
@@ -531,6 +531,42 @@
   </si>
   <si>
     <t>idx_plans_name</t>
+  </si>
+  <si>
+    <t>idx_plan_modalities</t>
+  </si>
+  <si>
+    <t>idx_plan_modalities_modality</t>
+  </si>
+  <si>
+    <t>idx_subscriptions</t>
+  </si>
+  <si>
+    <t>idx_subscriptions_plan</t>
+  </si>
+  <si>
+    <t>idx_subscriptions_active</t>
+  </si>
+  <si>
+    <t>idx_payment_method_name</t>
+  </si>
+  <si>
+    <t>idx_payments_subscription</t>
+  </si>
+  <si>
+    <t>idx_payments_dt</t>
+  </si>
+  <si>
+    <t>idx_payments_method</t>
+  </si>
+  <si>
+    <t>idx_classes_modality</t>
+  </si>
+  <si>
+    <t>idx_classes_instructor</t>
+  </si>
+  <si>
+    <t>idx_classes_dt</t>
   </si>
 </sst>
 </file>
@@ -653,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -694,15 +730,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -714,15 +741,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -756,9 +774,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -766,6 +781,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -776,15 +803,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1119,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A588904-58D6-4340-A48F-92FCD18181A8}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,47 +1153,47 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1196,10 +1214,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1218,10 +1236,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
@@ -1238,10 +1256,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="39"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1259,10 +1277,10 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="39"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1279,10 +1297,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="39"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1331,66 +1349,37 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="47"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="46" t="s">
+      <c r="F12" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="48"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-    </row>
+      <c r="G12" s="38"/>
+      <c r="H12" s="37"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -1414,128 +1403,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="26" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
+      <c r="E5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="26" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32" t="s">
+      <c r="E6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>125</v>
       </c>
       <c r="I7" s="10"/>
@@ -1557,36 +1546,36 @@
         <v>18</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1583,7 @@
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1630,229 +1619,229 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="26" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
+      <c r="E5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32" t="s">
+      <c r="E6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>131</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="26" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26" t="s">
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21" t="s">
+      <c r="E10" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="41" t="s">
         <v>138</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
+      <c r="E11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="41" t="s">
         <v>140</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21" t="s">
+      <c r="E12" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1873,40 +1862,40 @@
         <v>18</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="45"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38" t="s">
+      <c r="E15" s="31"/>
+      <c r="F15" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="17"/>
+      <c r="H29" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1934,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A1AA6A6-CB8B-4065-8215-EA9657872912}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,108 +1936,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="27" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="32" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="26" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
+      <c r="E5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="32" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="26" t="s">
         <v>146</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32" t="s">
+      <c r="E6" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26" t="s">
         <v>148</v>
       </c>
     </row>
@@ -2070,46 +2059,46 @@
         <v>18</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="35"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="52" t="s">
+      <c r="E9" s="25"/>
+      <c r="F9" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="54"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="30"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2131,7 +2120,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2146,47 +2135,47 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2207,10 +2196,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2229,10 +2218,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2282,67 +2271,56 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="38"/>
-      <c r="B9" s="38"/>
+      <c r="A9" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="35"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
+      <c r="F9" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
+      <c r="A10" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="35"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-    </row>
+      <c r="F10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="F11:H11"/>
+  <mergeCells count="10">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F10:H10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2354,7 +2332,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,47 +2347,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2430,10 +2408,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2452,10 +2430,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
@@ -2472,63 +2450,63 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>54</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="27" t="s">
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26" t="s">
+      <c r="E9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2558,69 +2536,82 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="37"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="47"/>
+      <c r="F12" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="36" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="37"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="15"/>
+      <c r="F13" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="46" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="48"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15"/>
-    </row>
+      <c r="F14" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F11:H11"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2631,7 +2622,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,47 +2637,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2707,10 +2698,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2729,10 +2720,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
@@ -2749,63 +2740,63 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>63</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="27" t="s">
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="29" t="s">
+      <c r="E9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2835,69 +2826,82 @@
       <c r="E11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="50"/>
-      <c r="H11" s="51"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="45"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="37"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="47"/>
+      <c r="F12" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15"/>
+      <c r="A13" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="48"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="6"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="15"/>
+      <c r="F13" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" s="37"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="15"/>
-    </row>
+      <c r="F14" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="37"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="16">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="F12:H12"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2908,7 +2912,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2923,47 +2927,47 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
@@ -2984,10 +2988,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="39"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
@@ -3006,10 +3010,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="39"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="8" t="s">
         <v>68</v>
       </c>
@@ -3052,54 +3056,32 @@
       <c r="E8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B9" s="37"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="E9" s="6"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="15"/>
-    </row>
+      <c r="F9" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="37"/>
+    </row>
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="30"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3109,10 +3091,12 @@
       </c>
     </row>
     <row r="30" spans="8:12" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="F9:H9"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -3143,128 +3127,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="E6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>81</v>
       </c>
       <c r="I7" s="10"/>
@@ -3286,36 +3270,36 @@
         <v>18</v>
       </c>
       <c r="B9" s="13"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="51"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3323,7 +3307,7 @@
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3359,108 +3343,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="E6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>41</v>
       </c>
     </row>
@@ -3482,76 +3466,76 @@
         <v>18</v>
       </c>
       <c r="B8" s="13"/>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="49" t="s">
+      <c r="F8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="45"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="46" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="47"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="37"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="46" t="s">
+      <c r="A10" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="B10" s="47"/>
+      <c r="B10" s="37"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="46" t="s">
+      <c r="E10" s="17"/>
+      <c r="F10" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="48"/>
-      <c r="H10" s="47"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="37"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I13" s="30"/>
+      <c r="I13" s="24"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F10:H10"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="F8:H8"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3562,7 +3546,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3574,149 +3558,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="15" t="s">
         <v>75</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="E6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="18" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18" t="s">
+      <c r="E7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>90</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="15" t="s">
         <v>92</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18" t="s">
+      <c r="E8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>93</v>
       </c>
     </row>
@@ -3737,13 +3721,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="13"/>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="16" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="11" t="s">
@@ -3753,58 +3737,71 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="36" t="s">
+        <v>171</v>
+      </c>
+      <c r="B11" s="37"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="37"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="24"/>
+      <c r="A12" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="37"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="24"/>
+      <c r="D12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="37"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
-      <c r="B13" s="24"/>
+      <c r="A13" s="36" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="37"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="24"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-    </row>
+      <c r="D13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="37"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="F14:H14"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -3827,289 +3824,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="16" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="18" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="18" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18" t="s">
+      <c r="E6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="26" t="s">
+      <c r="B7" s="40"/>
+      <c r="C7" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26" t="s">
+      <c r="E7" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20" t="s">
         <v>103</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="21" t="s">
+      <c r="B8" s="42"/>
+      <c r="C8" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="27" t="s">
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="21" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="43"/>
-      <c r="C9" s="26" t="s">
+      <c r="B9" s="40"/>
+      <c r="C9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="29" t="s">
+      <c r="E9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="26" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26" t="s">
+      <c r="E10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+    <row r="11" spans="1:9" s="30" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="26" t="s">
+      <c r="B11" s="40"/>
+      <c r="C11" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26" t="s">
+      <c r="E11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="21" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21" t="s">
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
+    <row r="13" spans="1:9" s="30" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="26" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26" t="s">
+      <c r="E13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
+    <row r="14" spans="1:9" s="30" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26" t="s">
+      <c r="E14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="36" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:9" s="30" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E15" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="29" t="s">
+      <c r="E15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="23" t="s">
         <v>120</v>
       </c>
     </row>
@@ -4130,90 +4127,98 @@
         <v>18</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="50"/>
-      <c r="H17" s="51"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="45"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="47"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E18" s="20"/>
-      <c r="F18" s="46" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="47"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="37"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="A19" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="B19" s="47"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="46" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="G19" s="48"/>
-      <c r="H19" s="47"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="37"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="46" t="s">
+      <c r="A20" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="46" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="47"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="37"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="B21" s="47"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="20"/>
-      <c r="F21" s="46" t="s">
+      <c r="E21" s="17"/>
+      <c r="F21" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="48"/>
-      <c r="H21" s="47"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="37"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H30" s="17"/>
+      <c r="H30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F21:H21"/>
@@ -4230,14 +4235,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: dicionario de dados
</commit_message>
<xml_diff>
--- a/dicionario_dados/dicionario_de_dados_cutegym.xlsx
+++ b/dicionario_dados/dicionario_de_dados_cutegym.xlsx
@@ -183,64 +183,64 @@
     <t xml:space="preserve">idx_plan_modalities_modality</t>
   </si>
   <si>
+    <t xml:space="preserve">subscriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela responsável por armazenar os dados das assinaturas dos alunos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_subscriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador da assinatura </t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código de identificador do usuário</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 a 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar se assinatura está ativa ou não</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dt_start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000-01-01 a 9999-12-31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data que foi feita a assinatura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idx_subscriptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idx_subscriptions_plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idx_subscriptions_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IX_subscriptions_active_dt_start_covering </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dt_start, active, id_plan, id_subscriptions </t>
+  </si>
+  <si>
     <t xml:space="preserve">IX_subscriptions_id_user_covering </t>
-  </si>
-  <si>
-    <t xml:space="preserve">subscriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tabela responsável por armazenar os dados das assinaturas dos alunos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_subscriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código de identificador da assinatura </t>
-  </si>
-  <si>
-    <t xml:space="preserve">id_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Código de identificador do usuário</t>
-  </si>
-  <si>
-    <t xml:space="preserve">active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 a 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificar se assinatura está ativa ou não</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dt_start</t>
-  </si>
-  <si>
-    <t xml:space="preserve">date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1000-01-01 a 9999-12-31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data que foi feita a assinatura</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idx_subscriptions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idx_subscriptions_plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idx_subscriptions_active</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IX_subscriptions_active_dt_start_covering </t>
-  </si>
-  <si>
-    <t xml:space="preserve">dt_start, active, id_plan, id_subscriptions </t>
   </si>
   <si>
     <t xml:space="preserve">id_user, id_plan, dt_start, active </t>
@@ -644,6 +644,7 @@
       <color theme="1" tint="0.15"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -736,100 +737,96 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1082,269 +1079,268 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="26.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="E9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="B1:H1"/>
@@ -1386,115 +1382,115 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>155</v>
       </c>
     </row>
@@ -1517,78 +1513,74 @@
       <c r="H7" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="10" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1628,115 +1620,115 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1759,7 +1751,7 @@
       <c r="H7" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
@@ -1862,56 +1854,55 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="11"/>
+      <c r="H29" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1954,176 +1945,172 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="18" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+    </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="I13" s="19"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2159,189 +2146,185 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2374,127 +2357,127 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13" t="s">
@@ -2509,40 +2492,40 @@
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="16" t="s">
-        <v>60</v>
+      <c r="H8" s="15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>14</v>
@@ -2550,123 +2533,123 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="19" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9" t="s">
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -2714,115 +2697,115 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2832,10 +2815,10 @@
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>14</v>
@@ -2845,7 +2828,7 @@
       <c r="H7" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
@@ -2863,7 +2846,7 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2888,103 +2871,103 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="10" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
@@ -3030,181 +3013,177 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="I13" s="19"/>
+    </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L20" s="0" t="s">
+      <c r="L20" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -3241,115 +3220,115 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>99</v>
       </c>
     </row>
@@ -3372,63 +3351,58 @@
       <c r="H7" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3466,192 +3440,188 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I13" s="20"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="I13" s="19"/>
+    </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3682,7 +3652,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
@@ -3690,241 +3660,239 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="35.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="B1:H1"/>
@@ -3965,115 +3933,115 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="3.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="A5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>125</v>
       </c>
     </row>
@@ -4096,7 +4064,7 @@
       <c r="H7" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
@@ -4114,20 +4082,20 @@
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="15" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>58</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>59</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>14</v>
@@ -4158,16 +4126,16 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" s="21" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" s="20" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
         <v>135</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>63</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>14</v>
@@ -4198,7 +4166,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" s="21" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="20" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
         <v>139</v>
       </c>
@@ -4218,7 +4186,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" s="21" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" s="20" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
         <v>143</v>
       </c>
@@ -4238,7 +4206,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="15" s="21" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="20" customFormat="true" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
         <v>145</v>
       </c>
@@ -4259,119 +4227,119 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="1" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F17" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="s">
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9" t="s">
+      <c r="B19" s="9"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9" t="s">
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9" t="s">
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="11"/>
+      <c r="H30" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="26">

</xml_diff>